<commit_message>
this is the last version before major changes, decided to make the algorithm and the loop on waiters instead of sections, trying to get priority waiters, so they will be assigned first
</commit_message>
<xml_diff>
--- a/Data/RotationCopy.xlsx
+++ b/Data/RotationCopy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gecexgokyuzu\Desktop\WaiterRotationApp\waiter_rotation_assigner\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF309550-3B90-47EA-91BD-E7EBF80FB513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE45EB9-3B9D-4358-BF65-2E63FDCF0C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="8685" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="975" yWindow="3660" windowWidth="15225" windowHeight="6645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cycle" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>SmokingSection</t>
+  </si>
+  <si>
+    <t>24/03/23</t>
   </si>
 </sst>
 </file>
@@ -459,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,6 +546,120 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
seperated the main loop into two phases by importance level. first phase gets the waiters the desired sections and second phase is for assigning a section to the last waiters, repetition will occur because uneven locations.
</commit_message>
<xml_diff>
--- a/Data/RotationCopy.xlsx
+++ b/Data/RotationCopy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gecexgokyuzu\Desktop\WaiterRotationApp\waiter_rotation_assigner\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE45EB9-3B9D-4358-BF65-2E63FDCF0C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD407CB-C037-413F-83A0-9B546C318222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="975" yWindow="3660" windowWidth="15225" windowHeight="6645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>SmokingSection</t>
-  </si>
-  <si>
-    <t>24/03/23</t>
   </si>
 </sst>
 </file>
@@ -462,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,120 +543,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>